<commit_message>
Writing new excel worksheet
</commit_message>
<xml_diff>
--- a/Data_Clean/City_Changes_Reported_Murders_2020_2023.xlsx
+++ b/Data_Clean/City_Changes_Reported_Murders_2020_2023.xlsx
@@ -546,13 +546,13 @@
         </is>
       </c>
       <c r="B12">
-        <v>33</v>
+        <v>30.75489282385834</v>
       </c>
       <c r="C12">
-        <v>30.75489282385834</v>
+        <v>25.98586704134461</v>
       </c>
       <c r="D12">
-        <v>-0.06803355079217147</v>
+        <v>-0.1550655958980979</v>
       </c>
     </row>
     <row r="13">
@@ -562,13 +562,13 @@
         </is>
       </c>
       <c r="B13">
-        <v>50.3</v>
+        <v>57.02947845804988</v>
       </c>
       <c r="C13">
-        <v>57.02947845804988</v>
+        <v>41.22492887372787</v>
       </c>
       <c r="D13">
-        <v>0.1337868480725623</v>
+        <v>-0.2771294778006365</v>
       </c>
     </row>
     <row r="14">
@@ -578,13 +578,13 @@
         </is>
       </c>
       <c r="B14">
-        <v>33.9</v>
+        <v>31.47632311977716</v>
       </c>
       <c r="C14">
-        <v>31.47632311977716</v>
+        <v>26.38881114407491</v>
       </c>
       <c r="D14">
-        <v>-0.07149489322191266</v>
+        <v>-0.1616298052457616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>